<commit_message>
added cash pickup and other api features
</commit_message>
<xml_diff>
--- a/cmd/web/static/files/TransactionBook.xlsx
+++ b/cmd/web/static/files/TransactionBook.xlsx
@@ -383,24 +383,24 @@
         <v>14</v>
       </c>
       <c r="D2" t="str">
-        <v>115666</v>
+        <v>8290781111</v>
       </c>
       <c r="E2" t="str"/>
       <c r="F2" t="str">
-        <v>281509</v>
+        <v>1156663232</v>
       </c>
       <c r="G2" t="str"/>
       <c r="H2">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="I2">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="J2" t="str">
-        <v>2023-12-16 13:32:23</v>
+        <v>2023-12-15 20:33:51</v>
       </c>
       <c r="K2" t="str">
-        <v>DR</v>
+        <v>INTERNAL TRANSFER FROM 829078 TO 115666</v>
       </c>
     </row>
     <row r="3">
@@ -414,24 +414,24 @@
         <v>14</v>
       </c>
       <c r="D3" t="str">
-        <v>115666</v>
+        <v>8290781111</v>
       </c>
       <c r="E3" t="str"/>
       <c r="F3" t="str">
-        <v>281509</v>
+        <v>1156663232</v>
       </c>
       <c r="G3" t="str"/>
       <c r="H3">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="I3">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="J3" t="str">
-        <v>2023-12-17 19:59:37</v>
+        <v>2023-12-15 20:35:51</v>
       </c>
       <c r="K3" t="str">
-        <v>DR</v>
+        <v>INTERNAL TRANSFER FROM 829078 TO 115666</v>
       </c>
     </row>
     <row r="4">
@@ -445,24 +445,179 @@
         <v>14</v>
       </c>
       <c r="D4" t="str">
-        <v>115666</v>
+        <v>8290781111</v>
       </c>
       <c r="E4" t="str"/>
       <c r="F4" t="str">
-        <v>281509</v>
+        <v>1156663232</v>
       </c>
       <c r="G4" t="str"/>
       <c r="H4">
+        <v>200</v>
+      </c>
+      <c r="I4">
+        <v>0.02</v>
+      </c>
+      <c r="J4" t="str">
+        <v>2023-12-15 20:50:27</v>
+      </c>
+      <c r="K4" t="str">
+        <v>INTERNAL TRANSFER FROM 829078 TO 115666</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5" t="str">
+        <v>pain</v>
+      </c>
+      <c r="C5">
+        <v>14</v>
+      </c>
+      <c r="D5" t="str">
+        <v>8290781111</v>
+      </c>
+      <c r="E5" t="str"/>
+      <c r="F5" t="str">
+        <v>1156663232</v>
+      </c>
+      <c r="G5" t="str"/>
+      <c r="H5">
         <v>500</v>
       </c>
-      <c r="I4">
+      <c r="I5">
         <v>0.05</v>
       </c>
-      <c r="J4" t="str">
-        <v>2023-12-17 21:58:10</v>
-      </c>
-      <c r="K4" t="str">
-        <v>DR</v>
+      <c r="J5" t="str">
+        <v>2023-12-17 22:06:51</v>
+      </c>
+      <c r="K5" t="str">
+        <v>INTERNAL TRANSFER FROM 829078 TO 115666</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6" t="str">
+        <v>pain</v>
+      </c>
+      <c r="C6">
+        <v>13</v>
+      </c>
+      <c r="D6" t="str">
+        <v>1156663232</v>
+      </c>
+      <c r="E6" t="str"/>
+      <c r="F6" t="str">
+        <v>2815091234</v>
+      </c>
+      <c r="G6" t="str"/>
+      <c r="H6">
+        <v>400</v>
+      </c>
+      <c r="I6">
+        <v>0.04</v>
+      </c>
+      <c r="J6" t="str">
+        <v>2023-12-17 22:08:28</v>
+      </c>
+      <c r="K6" t="str">
+        <v>INTERNAL TRANSFER FROM 115666 TO 281509</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7" t="str">
+        <v>pain</v>
+      </c>
+      <c r="C7">
+        <v>13</v>
+      </c>
+      <c r="D7" t="str">
+        <v>6475711616</v>
+      </c>
+      <c r="E7" t="str"/>
+      <c r="F7" t="str">
+        <v>2815091234</v>
+      </c>
+      <c r="G7" t="str"/>
+      <c r="H7">
+        <v>435</v>
+      </c>
+      <c r="I7">
+        <v>0.0435</v>
+      </c>
+      <c r="J7" t="str">
+        <v>2023-12-17 22:22:57</v>
+      </c>
+      <c r="K7" t="str">
+        <v>INTERNAL TRANSFER FROM 647571 TO 281509</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8" t="str">
+        <v>pain</v>
+      </c>
+      <c r="C8">
+        <v>13</v>
+      </c>
+      <c r="D8" t="str">
+        <v>6475711616</v>
+      </c>
+      <c r="E8" t="str"/>
+      <c r="F8" t="str">
+        <v>2815091234</v>
+      </c>
+      <c r="G8" t="str"/>
+      <c r="H8">
+        <v>500</v>
+      </c>
+      <c r="I8">
+        <v>0.05</v>
+      </c>
+      <c r="J8" t="str">
+        <v>2023-12-20 07:52:24</v>
+      </c>
+      <c r="K8" t="str">
+        <v>INTERNAL TRANSFER FROM 647571 TO 281509</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9" t="str">
+        <v>pain</v>
+      </c>
+      <c r="C9">
+        <v>14</v>
+      </c>
+      <c r="D9" t="str">
+        <v>8290781111</v>
+      </c>
+      <c r="E9" t="str"/>
+      <c r="F9" t="str">
+        <v>2815091234</v>
+      </c>
+      <c r="G9" t="str"/>
+      <c r="H9">
+        <v>500</v>
+      </c>
+      <c r="I9">
+        <v>0.05</v>
+      </c>
+      <c r="J9" t="str">
+        <v>2023-12-22 10:54:58</v>
+      </c>
+      <c r="K9" t="str">
+        <v>INTERNAL TRANSFER FROM 829078 TO 281509</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new priviledge feature to dashboard
</commit_message>
<xml_diff>
--- a/cmd/web/static/files/TransactionBook.xlsx
+++ b/cmd/web/static/files/TransactionBook.xlsx
@@ -383,11 +383,11 @@
         <v>14</v>
       </c>
       <c r="D2" t="str">
-        <v>8290781111</v>
+        <v>829078</v>
       </c>
       <c r="E2" t="str"/>
       <c r="F2" t="str">
-        <v>1156663232</v>
+        <v>115666</v>
       </c>
       <c r="G2" t="str"/>
       <c r="H2">
@@ -400,7 +400,7 @@
         <v>2023-12-15 20:33:51</v>
       </c>
       <c r="K2" t="str">
-        <v>INTERNAL TRANSFER FROM 829078 TO 115666</v>
+        <v>CR</v>
       </c>
     </row>
     <row r="3">
@@ -414,11 +414,11 @@
         <v>14</v>
       </c>
       <c r="D3" t="str">
-        <v>8290781111</v>
+        <v>829078</v>
       </c>
       <c r="E3" t="str"/>
       <c r="F3" t="str">
-        <v>1156663232</v>
+        <v>115666</v>
       </c>
       <c r="G3" t="str"/>
       <c r="H3">
@@ -431,7 +431,7 @@
         <v>2023-12-15 20:35:51</v>
       </c>
       <c r="K3" t="str">
-        <v>INTERNAL TRANSFER FROM 829078 TO 115666</v>
+        <v>CR</v>
       </c>
     </row>
     <row r="4">
@@ -445,24 +445,24 @@
         <v>14</v>
       </c>
       <c r="D4" t="str">
-        <v>8290781111</v>
+        <v>115666</v>
       </c>
       <c r="E4" t="str"/>
       <c r="F4" t="str">
-        <v>1156663232</v>
+        <v>829078</v>
       </c>
       <c r="G4" t="str"/>
       <c r="H4">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="I4">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="J4" t="str">
-        <v>2023-12-15 20:50:27</v>
+        <v>2023-12-15 20:36:34</v>
       </c>
       <c r="K4" t="str">
-        <v>INTERNAL TRANSFER FROM 829078 TO 115666</v>
+        <v>DR</v>
       </c>
     </row>
     <row r="5">
@@ -476,11 +476,11 @@
         <v>14</v>
       </c>
       <c r="D5" t="str">
-        <v>8290781111</v>
+        <v>115666</v>
       </c>
       <c r="E5" t="str"/>
       <c r="F5" t="str">
-        <v>1156663232</v>
+        <v>829078</v>
       </c>
       <c r="G5" t="str"/>
       <c r="H5">
@@ -490,10 +490,10 @@
         <v>0.05</v>
       </c>
       <c r="J5" t="str">
-        <v>2023-12-17 22:06:51</v>
+        <v>2023-12-15 20:36:36</v>
       </c>
       <c r="K5" t="str">
-        <v>INTERNAL TRANSFER FROM 829078 TO 115666</v>
+        <v>DR</v>
       </c>
     </row>
     <row r="6">
@@ -504,27 +504,27 @@
         <v>pain</v>
       </c>
       <c r="C6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" t="str">
-        <v>1156663232</v>
+        <v>829078</v>
       </c>
       <c r="E6" t="str"/>
       <c r="F6" t="str">
-        <v>2815091234</v>
+        <v>115666</v>
       </c>
       <c r="G6" t="str"/>
       <c r="H6">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="I6">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="J6" t="str">
-        <v>2023-12-17 22:08:28</v>
+        <v>2023-12-15 20:50:27</v>
       </c>
       <c r="K6" t="str">
-        <v>INTERNAL TRANSFER FROM 115666 TO 281509</v>
+        <v>CR</v>
       </c>
     </row>
     <row r="7">
@@ -535,27 +535,27 @@
         <v>pain</v>
       </c>
       <c r="C7">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" t="str">
-        <v>6475711616</v>
+        <v>829078</v>
       </c>
       <c r="E7" t="str"/>
       <c r="F7" t="str">
-        <v>2815091234</v>
+        <v>115666</v>
       </c>
       <c r="G7" t="str"/>
       <c r="H7">
-        <v>435</v>
+        <v>200</v>
       </c>
       <c r="I7">
-        <v>0.0435</v>
+        <v>0.02</v>
       </c>
       <c r="J7" t="str">
-        <v>2023-12-17 22:22:57</v>
+        <v>2023-12-17 21:55:50</v>
       </c>
       <c r="K7" t="str">
-        <v>INTERNAL TRANSFER FROM 647571 TO 281509</v>
+        <v>CR</v>
       </c>
     </row>
     <row r="8">
@@ -566,14 +566,14 @@
         <v>pain</v>
       </c>
       <c r="C8">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D8" t="str">
-        <v>6475711616</v>
+        <v>829078</v>
       </c>
       <c r="E8" t="str"/>
       <c r="F8" t="str">
-        <v>2815091234</v>
+        <v>115666</v>
       </c>
       <c r="G8" t="str"/>
       <c r="H8">
@@ -583,10 +583,10 @@
         <v>0.05</v>
       </c>
       <c r="J8" t="str">
-        <v>2023-12-20 07:52:24</v>
+        <v>2023-12-17 22:06:51</v>
       </c>
       <c r="K8" t="str">
-        <v>INTERNAL TRANSFER FROM 647571 TO 281509</v>
+        <v>CR</v>
       </c>
     </row>
     <row r="9">
@@ -600,24 +600,148 @@
         <v>14</v>
       </c>
       <c r="D9" t="str">
-        <v>8290781111</v>
+        <v>829078</v>
       </c>
       <c r="E9" t="str"/>
       <c r="F9" t="str">
-        <v>2815091234</v>
+        <v>115666</v>
       </c>
       <c r="G9" t="str"/>
       <c r="H9">
+        <v>10000</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9" t="str">
+        <v>2023-12-17 22:27:04</v>
+      </c>
+      <c r="K9" t="str">
+        <v>CR</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10" t="str">
+        <v>pain</v>
+      </c>
+      <c r="C10">
+        <v>14</v>
+      </c>
+      <c r="D10" t="str">
+        <v>829078</v>
+      </c>
+      <c r="E10" t="str"/>
+      <c r="F10" t="str">
+        <v>115666</v>
+      </c>
+      <c r="G10" t="str"/>
+      <c r="H10">
+        <v>1000</v>
+      </c>
+      <c r="I10">
+        <v>0.1</v>
+      </c>
+      <c r="J10" t="str">
+        <v>2023-12-17 22:53:57</v>
+      </c>
+      <c r="K10" t="str">
+        <v>CR</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11" t="str">
+        <v>pain</v>
+      </c>
+      <c r="C11">
+        <v>14</v>
+      </c>
+      <c r="D11" t="str">
+        <v>829078</v>
+      </c>
+      <c r="E11" t="str"/>
+      <c r="F11" t="str">
+        <v>441524</v>
+      </c>
+      <c r="G11" t="str"/>
+      <c r="H11">
         <v>500</v>
       </c>
-      <c r="I9">
+      <c r="I11">
         <v>0.05</v>
       </c>
-      <c r="J9" t="str">
-        <v>2023-12-22 10:54:58</v>
-      </c>
-      <c r="K9" t="str">
-        <v>INTERNAL TRANSFER FROM 829078 TO 281509</v>
+      <c r="J11" t="str">
+        <v>2023-12-17 22:54:54</v>
+      </c>
+      <c r="K11" t="str">
+        <v>CR</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12" t="str">
+        <v>pain</v>
+      </c>
+      <c r="C12">
+        <v>14</v>
+      </c>
+      <c r="D12" t="str">
+        <v>829078</v>
+      </c>
+      <c r="E12" t="str"/>
+      <c r="F12" t="str">
+        <v>115666</v>
+      </c>
+      <c r="G12" t="str"/>
+      <c r="H12">
+        <v>500</v>
+      </c>
+      <c r="I12">
+        <v>0.05</v>
+      </c>
+      <c r="J12" t="str">
+        <v>2023-12-18 12:59:35</v>
+      </c>
+      <c r="K12" t="str">
+        <v>CR</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13" t="str">
+        <v>pain</v>
+      </c>
+      <c r="C13">
+        <v>14</v>
+      </c>
+      <c r="D13" t="str">
+        <v>829078</v>
+      </c>
+      <c r="E13" t="str"/>
+      <c r="F13" t="str">
+        <v>441524</v>
+      </c>
+      <c r="G13" t="str"/>
+      <c r="H13">
+        <v>10000</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13" t="str">
+        <v>2023-12-18 13:20:54</v>
+      </c>
+      <c r="K13" t="str">
+        <v>DR</v>
       </c>
     </row>
   </sheetData>

</xml_diff>